<commit_message>
updated fig2 with vitamins
</commit_message>
<xml_diff>
--- a/data/nut/uk_vitamin_data.xlsx
+++ b/data/nut/uk_vitamin_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robins64/Documents/git_repos/ghg/data/nut/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D51DD1-40FA-0941-BB0F-FEEA365E8793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF54FB7-7A01-6943-AE8B-0AF5DA45BE99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3040" yWindow="2200" windowWidth="27640" windowHeight="16940" xr2:uid="{6EC324D1-8D18-1043-AC0B-DFCA1AA26B36}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="206">
   <si>
     <t>Food Code</t>
   </si>
@@ -647,6 +647,12 @@
   </si>
   <si>
     <t>1.00</t>
+  </si>
+  <si>
+    <t>04.053</t>
+  </si>
+  <si>
+    <t>Mussel, blue, raw</t>
   </si>
 </sst>
 </file>
@@ -699,7 +705,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -737,6 +743,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1051,10 +1058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB5009A3-981F-2E4B-93F1-FDF59C5FA1C6}">
-  <dimension ref="A1:Z14"/>
+  <dimension ref="A1:Z15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="Z16" sqref="Z16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2091,6 +2098,53 @@
         <v>192</v>
       </c>
     </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>195</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="J15" s="14">
+        <v>14</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" s="14">
+        <v>14</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="P15" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="14">
+        <v>0.27</v>
+      </c>
+      <c r="R15" s="14">
+        <v>1.2</v>
+      </c>
+      <c r="V15" s="14">
+        <v>25</v>
+      </c>
+      <c r="W15" s="14">
+        <v>42</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>